<commit_message>
added yr in front of years
</commit_message>
<xml_diff>
--- a/Reproducibility_Package/Excel_Files/VATdatasheet.xlsx
+++ b/Reproducibility_Package/Excel_Files/VATdatasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sumailsyr-my.sharepoint.com/personal/ujbilgra_syr_edu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sumailsyr-my.sharepoint.com/personal/kesarrge_syr_edu/Documents/ECN 310/course-project-taxes-tariffs/Reproducibility_Package/Excel_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D9155EC-2DD5-4199-9BC9-CE57F4DE9156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{3D9155EC-2DD5-4199-9BC9-CE57F4DE9156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC7CDA19-7769-48EE-8FA7-F2C6CD859CC0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21750" windowHeight="10740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="3000" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,111 +29,6 @@
     <t>Indicator Name</t>
   </si>
   <si>
-    <t>1988</t>
-  </si>
-  <si>
-    <t>1989</t>
-  </si>
-  <si>
-    <t>1990</t>
-  </si>
-  <si>
-    <t>1991</t>
-  </si>
-  <si>
-    <t>1992</t>
-  </si>
-  <si>
-    <t>1993</t>
-  </si>
-  <si>
-    <t>1994</t>
-  </si>
-  <si>
-    <t>1995</t>
-  </si>
-  <si>
-    <t>1996</t>
-  </si>
-  <si>
-    <t>1997</t>
-  </si>
-  <si>
-    <t>1998</t>
-  </si>
-  <si>
-    <t>1999</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>2001</t>
-  </si>
-  <si>
-    <t>2002</t>
-  </si>
-  <si>
-    <t>2003</t>
-  </si>
-  <si>
-    <t>2004</t>
-  </si>
-  <si>
-    <t>2005</t>
-  </si>
-  <si>
-    <t>2006</t>
-  </si>
-  <si>
-    <t>2007</t>
-  </si>
-  <si>
-    <t>2008</t>
-  </si>
-  <si>
-    <t>2009</t>
-  </si>
-  <si>
-    <t>2010</t>
-  </si>
-  <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
     <t>Afghanistan</t>
   </si>
   <si>
@@ -714,16 +609,127 @@
   </si>
   <si>
     <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>yr1988</t>
+  </si>
+  <si>
+    <t>yr1989</t>
+  </si>
+  <si>
+    <t>yr1990</t>
+  </si>
+  <si>
+    <t>yr1991</t>
+  </si>
+  <si>
+    <t>yr1992</t>
+  </si>
+  <si>
+    <t>yr1993</t>
+  </si>
+  <si>
+    <t>yr1994</t>
+  </si>
+  <si>
+    <t>yr1995</t>
+  </si>
+  <si>
+    <t>yr1996</t>
+  </si>
+  <si>
+    <t>yr1997</t>
+  </si>
+  <si>
+    <t>yr1998</t>
+  </si>
+  <si>
+    <t>yr1999</t>
+  </si>
+  <si>
+    <t>yr2000</t>
+  </si>
+  <si>
+    <t>yr2001</t>
+  </si>
+  <si>
+    <t>yr2002</t>
+  </si>
+  <si>
+    <t>yr2003</t>
+  </si>
+  <si>
+    <t>yr2004</t>
+  </si>
+  <si>
+    <t>yr2005</t>
+  </si>
+  <si>
+    <t>yr2006</t>
+  </si>
+  <si>
+    <t>yr2007</t>
+  </si>
+  <si>
+    <t>yr2008</t>
+  </si>
+  <si>
+    <t>yr2009</t>
+  </si>
+  <si>
+    <t>yr2010</t>
+  </si>
+  <si>
+    <t>yr2011</t>
+  </si>
+  <si>
+    <t>yr2012</t>
+  </si>
+  <si>
+    <t>yr2013</t>
+  </si>
+  <si>
+    <t>yr2014</t>
+  </si>
+  <si>
+    <t>yr2015</t>
+  </si>
+  <si>
+    <t>yr2016</t>
+  </si>
+  <si>
+    <t>yr2017</t>
+  </si>
+  <si>
+    <t>yr2018</t>
+  </si>
+  <si>
+    <t>yr2019</t>
+  </si>
+  <si>
+    <t>yr2020</t>
+  </si>
+  <si>
+    <t>yr2021</t>
+  </si>
+  <si>
+    <t>yr2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1067,7 +1073,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AL5" sqref="AL5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1085,117 +1093,117 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>196</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>197</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>198</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>199</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>201</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>202</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>203</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>204</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>205</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>206</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>207</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>208</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
+        <v>210</v>
       </c>
       <c r="R1" t="s">
-        <v>17</v>
+        <v>211</v>
       </c>
       <c r="S1" t="s">
-        <v>18</v>
+        <v>212</v>
       </c>
       <c r="T1" t="s">
-        <v>19</v>
+        <v>213</v>
       </c>
       <c r="U1" t="s">
-        <v>20</v>
+        <v>214</v>
       </c>
       <c r="V1" t="s">
-        <v>21</v>
+        <v>215</v>
       </c>
       <c r="W1" t="s">
-        <v>22</v>
+        <v>216</v>
       </c>
       <c r="X1" t="s">
-        <v>23</v>
+        <v>217</v>
       </c>
       <c r="Y1" t="s">
-        <v>24</v>
+        <v>218</v>
       </c>
       <c r="Z1" t="s">
-        <v>25</v>
+        <v>219</v>
       </c>
       <c r="AA1" t="s">
-        <v>26</v>
+        <v>220</v>
       </c>
       <c r="AB1" t="s">
-        <v>27</v>
+        <v>221</v>
       </c>
       <c r="AC1" t="s">
-        <v>28</v>
+        <v>222</v>
       </c>
       <c r="AD1" t="s">
-        <v>29</v>
+        <v>223</v>
       </c>
       <c r="AE1" t="s">
-        <v>30</v>
+        <v>224</v>
       </c>
       <c r="AF1" t="s">
-        <v>31</v>
+        <v>225</v>
       </c>
       <c r="AG1" t="s">
-        <v>32</v>
+        <v>226</v>
       </c>
       <c r="AH1" t="s">
-        <v>33</v>
+        <v>227</v>
       </c>
       <c r="AI1" t="s">
-        <v>34</v>
+        <v>228</v>
       </c>
       <c r="AJ1" t="s">
-        <v>35</v>
+        <v>229</v>
       </c>
       <c r="AK1" t="s">
-        <v>36</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="U2">
         <v>2.5137170930119201</v>
@@ -1236,10 +1244,10 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <v>8.3470058720705094</v>
@@ -1295,26 +1303,26 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="N6">
         <v>2.0282171071848101</v>
@@ -1382,18 +1390,18 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>2.4828260323967801</v>
@@ -1494,10 +1502,10 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AA9">
         <v>13.259242892853999</v>
@@ -1532,18 +1540,18 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>5.9256855245966298</v>
@@ -1644,10 +1652,10 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>10.2854372500379</v>
@@ -1754,10 +1762,10 @@
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="I13">
         <v>11.868637216747</v>
@@ -1822,10 +1830,10 @@
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="G14">
         <v>1.0038526767770799</v>
@@ -1920,18 +1928,18 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="P16">
         <v>3.1230427259966498</v>
@@ -1999,10 +2007,10 @@
     </row>
     <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="R17">
         <v>13.264590607852901</v>
@@ -2049,10 +2057,10 @@
     </row>
     <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="G18">
         <v>17.164179104477601</v>
@@ -2144,10 +2152,10 @@
     </row>
     <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J19">
         <v>11.893899487947399</v>
@@ -2233,10 +2241,10 @@
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <v>2.4349846952688199</v>
@@ -2325,26 +2333,26 @@
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>6.5039897173518399</v>
@@ -2448,10 +2456,10 @@
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C24">
         <v>6.1245692382497596</v>
@@ -2516,10 +2524,10 @@
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="T25">
         <v>10.6919262579818</v>
@@ -2575,10 +2583,10 @@
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E26">
         <v>1.1202109384363399</v>
@@ -2652,10 +2660,10 @@
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="Y27">
         <v>8.3014163720190695</v>
@@ -2696,18 +2704,18 @@
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E29">
         <v>9.8718569281328801</v>
@@ -2808,10 +2816,10 @@
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="Q30">
         <v>7.7050610080709001</v>
@@ -2876,10 +2884,10 @@
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="F31">
         <v>16.630305548822001</v>
@@ -2911,10 +2919,10 @@
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="Q32">
         <v>6.5948257421652201</v>
@@ -2979,10 +2987,10 @@
     </row>
     <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E33">
         <v>4.3080474895449399</v>
@@ -3041,10 +3049,10 @@
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="L34">
         <v>3.9243840861676502</v>
@@ -3118,10 +3126,10 @@
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="T35">
         <v>15.988873956637701</v>
@@ -3165,18 +3173,18 @@
     </row>
     <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AH37">
         <v>5.9066514070798997</v>
@@ -3190,18 +3198,18 @@
     </row>
     <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C39">
         <v>10.0246349560373</v>
@@ -3308,10 +3316,10 @@
     </row>
     <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="T40">
         <v>8.79682467490648</v>
@@ -3367,10 +3375,10 @@
     </row>
     <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="M41">
         <v>5.8811581577118099</v>
@@ -3423,26 +3431,26 @@
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="P44">
         <v>7.3853329878206804</v>
@@ -3507,10 +3515,10 @@
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C45">
         <v>5.5650668522385898</v>
@@ -3611,10 +3619,10 @@
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E46">
         <v>9.3762697267650594</v>
@@ -3688,10 +3696,10 @@
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J47">
         <v>2.67497152021269</v>
@@ -3777,18 +3785,18 @@
     </row>
     <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J49">
         <v>16.147214439994102</v>
@@ -3874,10 +3882,10 @@
     </row>
     <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="H50">
         <v>11.9966546495194</v>
@@ -3969,10 +3977,10 @@
     </row>
     <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C51">
         <v>20.2871212339879</v>
@@ -4079,26 +4087,26 @@
     </row>
     <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C54">
         <v>4.0745626266356796</v>
@@ -4205,10 +4213,10 @@
     </row>
     <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="Y55">
         <v>5.6488182229626398</v>
@@ -4249,10 +4257,10 @@
     </row>
     <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AB56">
         <v>8.73792132749624</v>
@@ -4284,10 +4292,10 @@
     </row>
     <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C57">
         <v>4.6028538666318104</v>
@@ -4364,10 +4372,10 @@
     </row>
     <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="M58">
         <v>6.9936068182494697</v>
@@ -4444,18 +4452,18 @@
     </row>
     <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J60">
         <v>14.459508904845601</v>
@@ -4541,18 +4549,18 @@
     </row>
     <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E62">
         <v>6.6804025393602799</v>
@@ -4647,18 +4655,18 @@
     </row>
     <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E64">
         <v>5.5949335882032196</v>
@@ -4738,10 +4746,10 @@
     </row>
     <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C65">
         <v>17.9653061147249</v>
@@ -4848,10 +4856,10 @@
     </row>
     <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="M66">
         <v>5.6630142016722802</v>
@@ -4886,10 +4894,10 @@
     </row>
     <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C67">
         <v>13.383913032859599</v>
@@ -4996,18 +5004,18 @@
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AA69">
         <v>2.5761023178982398</v>
@@ -5036,10 +5044,10 @@
     </row>
     <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E70">
         <v>9.6013548978311203</v>
@@ -5047,10 +5055,10 @@
     </row>
     <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="K71">
         <v>6.2660565189466899</v>
@@ -5133,10 +5141,10 @@
     </row>
     <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="F72">
         <v>7.6291731905651803</v>
@@ -5234,10 +5242,10 @@
     </row>
     <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E73">
         <v>6.8304460042476602</v>
@@ -5314,10 +5322,10 @@
     </row>
     <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J74">
         <v>14.1039542000207</v>
@@ -5403,26 +5411,26 @@
     </row>
     <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E77">
         <v>4.4893854411422298</v>
@@ -5523,10 +5531,10 @@
     </row>
     <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E78">
         <v>3.2314660068316199</v>
@@ -5540,10 +5548,10 @@
     </row>
     <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AF79">
         <v>9.53222202249197</v>
@@ -5554,18 +5562,18 @@
     </row>
     <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="R81">
         <v>11.2638893924969</v>
@@ -5612,18 +5620,18 @@
     </row>
     <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J83">
         <v>15.6765021794841</v>
@@ -5709,10 +5717,10 @@
     </row>
     <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="B84" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J84">
         <v>20.017631456724001</v>
@@ -5798,10 +5806,10 @@
     </row>
     <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C85">
         <v>7.2737281487091101</v>
@@ -5899,10 +5907,10 @@
     </row>
     <row r="86" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="B86" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C86">
         <v>5.4670968871583803</v>
@@ -5997,10 +6005,10 @@
     </row>
     <row r="87" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="B87" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C87">
         <v>1.38823500736784</v>
@@ -6071,10 +6079,10 @@
     </row>
     <row r="88" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AC88">
         <v>0.10405173180548</v>
@@ -6097,10 +6105,10 @@
     </row>
     <row r="89" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="B89" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J89">
         <v>14.844183453669499</v>
@@ -6186,10 +6194,10 @@
     </row>
     <row r="90" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B90" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J90">
         <v>13.1475737416533</v>
@@ -6275,10 +6283,10 @@
     </row>
     <row r="91" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="B91" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E91">
         <v>12.2311564800815</v>
@@ -6379,10 +6387,10 @@
     </row>
     <row r="92" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="B92" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="H92">
         <v>10.4137861034515</v>
@@ -6471,18 +6479,18 @@
     </row>
     <row r="93" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="B93" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="B94" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E94">
         <v>7.1730486645345302</v>
@@ -6580,10 +6588,10 @@
     </row>
     <row r="95" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="L95">
         <v>4.8118269141188401</v>
@@ -6648,10 +6656,10 @@
     </row>
     <row r="96" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AC96">
         <v>7.8466774999830102</v>
@@ -6677,10 +6685,10 @@
     </row>
     <row r="97" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="Z97">
         <v>5.7335728538619998E-2</v>
@@ -6715,10 +6723,10 @@
     </row>
     <row r="98" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C98">
         <v>7.2916131715444399</v>
@@ -6825,18 +6833,18 @@
     </row>
     <row r="99" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="B99" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="B100" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AC100">
         <v>14.2820341976372</v>
@@ -6865,18 +6873,18 @@
     </row>
     <row r="101" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="B102" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J102">
         <v>19.826091089532</v>
@@ -6962,10 +6970,10 @@
     </row>
     <row r="103" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="B103" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="O103">
         <v>5.0294769608074299</v>
@@ -7036,10 +7044,10 @@
     </row>
     <row r="104" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="B104" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C104">
         <v>10.973777665595399</v>
@@ -7143,18 +7151,18 @@
     </row>
     <row r="105" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="B105" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="B106" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J106">
         <v>13.3382866972659</v>
@@ -7240,10 +7248,10 @@
     </row>
     <row r="107" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="B107" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J107">
         <v>12.7843546684387</v>
@@ -7329,10 +7337,10 @@
     </row>
     <row r="108" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="B108" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="K108">
         <v>11.8018196950781</v>
@@ -7415,10 +7423,10 @@
     </row>
     <row r="109" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="B109" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="V109">
         <v>4.19610400434519</v>
@@ -7468,10 +7476,10 @@
     </row>
     <row r="110" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="X110">
         <v>7.0231280766766897</v>
@@ -7515,10 +7523,10 @@
     </row>
     <row r="111" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="K111">
         <v>6.8823711980136597</v>
@@ -7601,10 +7609,10 @@
     </row>
     <row r="112" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="B112" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="R112">
         <v>3.43031759875266</v>
@@ -7630,10 +7638,10 @@
     </row>
     <row r="113" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="O113">
         <v>11.289126555393199</v>
@@ -7701,10 +7709,10 @@
     </row>
     <row r="114" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C114">
         <v>2.5768629724813299</v>
@@ -7811,18 +7819,18 @@
     </row>
     <row r="115" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="B115" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>152</v>
+        <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C116">
         <v>7.0028037383177599</v>
@@ -7929,10 +7937,10 @@
     </row>
     <row r="117" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C117">
         <v>10.4643615227194</v>
@@ -8018,10 +8026,10 @@
     </row>
     <row r="118" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>154</v>
+        <v>119</v>
       </c>
       <c r="B118" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="W118">
         <v>1.97248439347535</v>
@@ -8065,10 +8073,10 @@
     </row>
     <row r="119" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="B119" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="K119">
         <v>14.328360335995001</v>
@@ -8151,10 +8159,10 @@
     </row>
     <row r="120" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="G120">
         <v>6.9826304697864297</v>
@@ -8240,18 +8248,18 @@
     </row>
     <row r="121" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="B121" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="B122" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E122">
         <v>12.4193023563642</v>
@@ -8343,10 +8351,10 @@
     </row>
     <row r="123" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="B123" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="Y123">
         <v>13.2774546193451</v>
@@ -8387,10 +8395,10 @@
     </row>
     <row r="124" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="B124" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AA124">
         <v>3.3933027623493</v>
@@ -8419,10 +8427,10 @@
     </row>
     <row r="125" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="B125" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E125">
         <v>8.0093346643766701</v>
@@ -8502,10 +8510,10 @@
     </row>
     <row r="126" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="B126" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E126">
         <v>7.3759465290409896</v>
@@ -8606,10 +8614,10 @@
     </row>
     <row r="127" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="B127" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C127">
         <v>11.560868212140001</v>
@@ -8716,18 +8724,18 @@
     </row>
     <row r="128" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="B128" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="B129" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C129">
         <v>11.5517942875743</v>
@@ -8795,10 +8803,10 @@
     </row>
     <row r="130" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="B130" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="I130">
         <v>7.2880183970996697</v>
@@ -8887,26 +8895,26 @@
     </row>
     <row r="131" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="B131" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="B132" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="B133" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="T133">
         <v>17.236122749630599</v>
@@ -8962,10 +8970,10 @@
     </row>
     <row r="134" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="B134" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C134">
         <v>18.2097709139911</v>
@@ -9072,10 +9080,10 @@
     </row>
     <row r="135" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="B135" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="T135">
         <v>3.3435026745959702</v>
@@ -9131,18 +9139,18 @@
     </row>
     <row r="136" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="B136" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="B137" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C137">
         <v>8.7974811649612104</v>
@@ -9165,10 +9173,10 @@
     </row>
     <row r="138" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="B138" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="W138">
         <v>8.9374548481007299</v>
@@ -9212,10 +9220,10 @@
     </row>
     <row r="139" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="B139" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AC139">
         <v>5.3148752170773896</v>
@@ -9244,10 +9252,10 @@
     </row>
     <row r="140" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="B140" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AC140">
         <v>6.5329344594270298</v>
@@ -9273,10 +9281,10 @@
     </row>
     <row r="141" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="B141" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="T141">
         <v>6.4011414702149798</v>
@@ -9332,10 +9340,10 @@
     </row>
     <row r="142" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="B142" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="F142">
         <v>8.7643108560633003</v>
@@ -9433,10 +9441,10 @@
     </row>
     <row r="143" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="B143" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E143">
         <v>5.4697586282048896</v>
@@ -9537,10 +9545,10 @@
     </row>
     <row r="144" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="B144" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J144">
         <v>13.1697274091949</v>
@@ -9626,10 +9634,10 @@
     </row>
     <row r="145" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="B145" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J145">
         <v>13.502455146262699</v>
@@ -9715,18 +9723,18 @@
     </row>
     <row r="146" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="B146" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="B147" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E147">
         <v>16.039933444259599</v>
@@ -9827,10 +9835,10 @@
     </row>
     <row r="148" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="B148" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="N148">
         <v>8.6437256023272599</v>
@@ -9904,10 +9912,10 @@
     </row>
     <row r="149" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="B149" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E149">
         <v>5.4525380712219897</v>
@@ -9942,10 +9950,10 @@
     </row>
     <row r="150" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="B150" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AA150">
         <v>15.665625256208401</v>
@@ -9980,18 +9988,18 @@
     </row>
     <row r="151" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="B151" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="B152" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="Y152">
         <v>1.1422865325802001</v>
@@ -10029,10 +10037,10 @@
     </row>
     <row r="153" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="B153" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AD153">
         <v>11.596685905857299</v>
@@ -10052,10 +10060,10 @@
     </row>
     <row r="154" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
       <c r="B154" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="V154">
         <v>20.120500145559099</v>
@@ -10105,10 +10113,10 @@
     </row>
     <row r="155" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="B155" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="H155">
         <v>4.1302292125644904</v>
@@ -10185,18 +10193,18 @@
     </row>
     <row r="156" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="B156" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="B157" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C157">
         <v>5.31023247761006</v>
@@ -10303,10 +10311,10 @@
     </row>
     <row r="158" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="B158" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J158">
         <v>14.8578703882261</v>
@@ -10392,10 +10400,10 @@
     </row>
     <row r="159" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="B159" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="J159">
         <v>14.329740536327</v>
@@ -10481,10 +10489,10 @@
     </row>
     <row r="160" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>196</v>
+        <v>161</v>
       </c>
       <c r="B160" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="Z160">
         <v>10.3059956377866</v>
@@ -10519,10 +10527,10 @@
     </row>
     <row r="161" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
       <c r="B161" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C161">
         <v>9.0663785836780999</v>
@@ -10629,10 +10637,10 @@
     </row>
     <row r="162" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="B162" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AA162">
         <v>7.8432115662817603</v>
@@ -10667,10 +10675,10 @@
     </row>
     <row r="163" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>199</v>
+        <v>164</v>
       </c>
       <c r="B163" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E163">
         <v>13.3047369570964</v>
@@ -10771,10 +10779,10 @@
     </row>
     <row r="164" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="B164" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E164">
         <v>1.2559737746356501</v>
@@ -10851,10 +10859,10 @@
     </row>
     <row r="165" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
       <c r="B165" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="U165">
         <v>3.6153094535035701</v>
@@ -10895,10 +10903,10 @@
     </row>
     <row r="166" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="B166" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E166">
         <v>4.1881504226544601</v>
@@ -10987,18 +10995,18 @@
     </row>
     <row r="167" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="B167" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="168" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>204</v>
+        <v>169</v>
       </c>
       <c r="B168" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C168">
         <v>13.3543863919329</v>
@@ -11105,10 +11113,10 @@
     </row>
     <row r="169" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
       <c r="B169" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E169">
         <v>4.9148656595474103</v>
@@ -11209,18 +11217,18 @@
     </row>
     <row r="170" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="B170" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>207</v>
+        <v>172</v>
       </c>
       <c r="B171" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="M171">
         <v>8.8464423513917101</v>
@@ -11246,10 +11254,10 @@
     </row>
     <row r="172" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>208</v>
+        <v>173</v>
       </c>
       <c r="B172" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="X172">
         <v>8.8148104301958092</v>
@@ -11284,10 +11292,10 @@
     </row>
     <row r="173" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>209</v>
+        <v>174</v>
       </c>
       <c r="B173" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="H173">
         <v>7.8541160462953803</v>
@@ -11379,10 +11387,10 @@
     </row>
     <row r="174" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="B174" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="S174">
         <v>4.0732180514252203</v>
@@ -11435,18 +11443,18 @@
     </row>
     <row r="175" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
       <c r="B175" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
       <c r="B176" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="P176">
         <v>6.4000708005066702</v>
@@ -11505,10 +11513,10 @@
     </row>
     <row r="177" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
       <c r="B177" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C177">
         <v>9.5837855188542207</v>
@@ -11588,10 +11596,10 @@
     </row>
     <row r="178" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>214</v>
+        <v>179</v>
       </c>
       <c r="B178" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C178">
         <v>5.4446945296909401</v>
@@ -11671,34 +11679,34 @@
     </row>
     <row r="179" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>215</v>
+        <v>180</v>
       </c>
       <c r="B179" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="180" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>216</v>
+        <v>181</v>
       </c>
       <c r="B180" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
       <c r="B181" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="182" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>218</v>
+        <v>183</v>
       </c>
       <c r="B182" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="AD182">
         <v>8.2992992617632506</v>
@@ -11724,10 +11732,10 @@
     </row>
     <row r="183" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>219</v>
+        <v>184</v>
       </c>
       <c r="B183" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="N183">
         <v>12.256197902662</v>
@@ -11801,10 +11809,10 @@
     </row>
     <row r="184" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>220</v>
+        <v>185</v>
       </c>
       <c r="B184" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="L184">
         <v>1.0126296638436201</v>
@@ -11851,10 +11859,10 @@
     </row>
     <row r="185" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="B185" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E185">
         <v>9.7043840006801094</v>
@@ -11955,10 +11963,10 @@
     </row>
     <row r="186" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="B186" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="L186">
         <v>0.68839104807400497</v>
@@ -12038,10 +12046,10 @@
     </row>
     <row r="187" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="B187" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="C187">
         <v>10.703271407006801</v>
@@ -12145,10 +12153,10 @@
     </row>
     <row r="188" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="B188" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="Z188">
         <v>10.4348810286362</v>
@@ -12183,10 +12191,10 @@
     </row>
     <row r="189" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>225</v>
+        <v>190</v>
       </c>
       <c r="B189" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="X189">
         <v>14.253042108027699</v>
@@ -12221,34 +12229,34 @@
     </row>
     <row r="190" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>226</v>
+        <v>191</v>
       </c>
       <c r="B190" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="191" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>227</v>
+        <v>192</v>
       </c>
       <c r="B191" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="192" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>228</v>
+        <v>193</v>
       </c>
       <c r="B192" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>229</v>
+        <v>194</v>
       </c>
       <c r="B193" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E193">
         <v>11.044790013007001</v>
@@ -12340,10 +12348,10 @@
     </row>
     <row r="194" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>230</v>
+        <v>195</v>
       </c>
       <c r="B194" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="X194">
         <v>3.9051952523914202</v>
@@ -12371,6 +12379,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>